<commit_message>
:construction: Se crea el servicio de delete, read y se cuadra los script correspondientes
</commit_message>
<xml_diff>
--- a/tests/data/testData.xlsx
+++ b/tests/data/testData.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>Username</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>Vargas</t>
+  </si>
+  <si>
+    <t>false</t>
   </si>
 </sst>
 </file>
@@ -645,7 +648,7 @@
         <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="F3" t="s">
         <v>18</v>

</xml_diff>